<commit_message>
Readme, changes, minor data changes - see new files.
</commit_message>
<xml_diff>
--- a/data/dota-data.xlsx
+++ b/data/dota-data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gasabr/Desktop/Machine Learning/dota2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gasabr/Desktop/Machine Learning/AtoD/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="460" windowWidth="22840" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="5960" yWindow="460" windowWidth="22840" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Clockwerk</t>
   </si>
   <si>
-    <t>CM</t>
-  </si>
-  <si>
     <t>Dark Seer</t>
   </si>
   <si>
@@ -420,6 +417,9 @@
   </si>
   <si>
     <t>Chaos Knight</t>
+  </si>
+  <si>
+    <t>Cristal Mayden</t>
   </si>
 </sst>
 </file>
@@ -746,8 +746,8 @@
   <dimension ref="A1:Z112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,37 +767,37 @@
   <sheetData>
     <row r="1" spans="1:26" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>6</v>
@@ -827,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <v>68</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6">
         <v>113</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <v>65</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12">
         <v>62</v>
@@ -1415,10 +1415,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17">
         <v>81</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>55</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>50</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24">
         <v>43</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>87</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>69</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27">
         <v>49</v>
@@ -1899,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R27">
         <v>3</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>107</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30">
         <v>7</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31">
         <v>103</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32">
         <v>106</v>
@@ -2112,7 +2112,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>58</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35">
         <v>41</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36">
         <v>72</v>
@@ -2276,7 +2276,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37">
         <v>59</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38">
         <v>74</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <v>91</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>64</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>8</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42">
         <v>90</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43">
         <v>23</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44">
         <v>104</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <v>52</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>31</v>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47">
         <v>54</v>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48">
         <v>25</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49">
         <v>26</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50">
         <v>80</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51">
         <v>48</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52">
         <v>77</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53">
         <v>97</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54">
         <v>94</v>
@@ -3014,7 +3014,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55">
         <v>82</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56">
         <v>9</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57">
         <v>10</v>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <v>89</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B59">
         <v>53</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60">
         <v>36</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61">
         <v>60</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62">
         <v>88</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63">
         <v>84</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64">
         <v>57</v>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65">
         <v>111</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66">
         <v>76</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67">
         <v>44</v>
@@ -3547,7 +3547,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68">
         <v>12</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69">
         <v>110</v>
@@ -3629,7 +3629,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70">
         <v>13</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71">
         <v>14</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B72">
         <v>45</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B73">
         <v>39</v>
@@ -3793,7 +3793,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74">
         <v>15</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B75">
         <v>32</v>
@@ -3875,7 +3875,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B76">
         <v>86</v>
@@ -3916,7 +3916,7 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -3957,7 +3957,7 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B78">
         <v>79</v>
@@ -3998,7 +3998,7 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B79">
         <v>11</v>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B80">
         <v>27</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B81">
         <v>75</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B82">
         <v>101</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83">
         <v>28</v>
@@ -4203,7 +4203,7 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84">
         <v>93</v>
@@ -4244,7 +4244,7 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B85">
         <v>35</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86">
         <v>67</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87">
         <v>71</v>
@@ -4367,7 +4367,7 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88">
         <v>17</v>
@@ -4408,7 +4408,7 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89">
         <v>18</v>
@@ -4449,7 +4449,7 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90">
         <v>105</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91">
         <v>46</v>
@@ -4531,7 +4531,7 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B92">
         <v>109</v>
@@ -4564,7 +4564,7 @@
         <v>0</v>
       </c>
       <c r="L92" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R92">
         <v>3</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B93">
         <v>29</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B94">
         <v>98</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B95">
         <v>34</v>
@@ -4695,7 +4695,7 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B96">
         <v>19</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B97">
         <v>83</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B98">
         <v>95</v>
@@ -4818,7 +4818,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99">
         <v>100</v>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B100">
         <v>85</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B101">
         <v>70</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B102">
         <v>20</v>
@@ -4982,7 +4982,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B103">
         <v>40</v>
@@ -5023,7 +5023,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B104">
         <v>47</v>
@@ -5064,7 +5064,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B105">
         <v>92</v>
@@ -5105,7 +5105,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106">
         <v>37</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107">
         <v>63</v>
@@ -5187,7 +5187,7 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B108">
         <v>21</v>
@@ -5228,7 +5228,7 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B109">
         <v>112</v>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B110">
         <v>30</v>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B111">
         <v>42</v>
@@ -5351,7 +5351,7 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B112">
         <v>22</v>

</xml_diff>